<commit_message>
Adding code for ego network activity. Updating some slides.
</commit_message>
<xml_diff>
--- a/activities/ego_networks/ego_atts.xlsx
+++ b/activities/ego_networks/ego_atts.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">age</t>
   </si>
   <si>
-    <t xml:space="preserve">kin?</t>
+    <t xml:space="preserve">is.kin</t>
   </si>
   <si>
     <t xml:space="preserve">Kedra</t>
@@ -86,6 +86,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -150,11 +151,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,188 +179,196 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5:F9"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="F2" s="1" t="b">
+      <c r="F2" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="b">
+      <c r="F3" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F4" s="1" t="b">
+      <c r="F4" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="F5" s="1" t="b">
+      <c r="F5" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="F6" s="1" t="b">
+      <c r="F6" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="b">
+      <c r="F7" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="0" t="n">
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="F8" s="1" t="b">
+      <c r="F8" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="C9" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="F9" s="1" t="b">
+      <c r="F9" s="2" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating to week 7
</commit_message>
<xml_diff>
--- a/activities/ego_networks/ego_atts.xlsx
+++ b/activities/ego_networks/ego_atts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -52,18 +52,15 @@
     <t xml:space="preserve">Rebecca</t>
   </si>
   <si>
-    <t xml:space="preserve">Curtis</t>
+    <t xml:space="preserve">Christina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
-    <t xml:space="preserve">Christina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lisa</t>
   </si>
   <si>
@@ -71,6 +68,21 @@
   </si>
   <si>
     <t xml:space="preserve">Tyler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seungyoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">William</t>
   </si>
 </sst>
 </file>
@@ -176,13 +188,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -233,7 +245,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -251,37 +263,37 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="F4" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -293,16 +305,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -323,7 +335,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -335,7 +347,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>16</v>
@@ -344,7 +356,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -352,23 +364,82 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="F11" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C9" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <f aca="false">TRUE()</f>
+      <c r="F12" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>